<commit_message>
fiksa ticket send, lagde starten på cookies
</commit_message>
<xml_diff>
--- a/risk/risikodiagram.xlsx
+++ b/risk/risikodiagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dashboard\terminoppgave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dashboard\terminoppgave\risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EA4E99-A22C-4553-92AE-E53FEE12FDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7594A231-4979-4BC9-97DB-DE948DC9904E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A95F7586-F3C1-4EE9-9421-CE44EA819227}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{A95F7586-F3C1-4EE9-9421-CE44EA819227}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Ikke sansynlig</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Søler vann på server</t>
+  </si>
+  <si>
+    <t>responsiv, detektiv , prevantiv</t>
   </si>
 </sst>
 </file>
@@ -193,14 +196,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0929F94B-020B-469F-B623-0BA5CAFE82FB}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="C469" sqref="C469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,13 +536,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -614,14 +617,14 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -717,7 +720,9 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>

</xml_diff>